<commit_message>
fixed initial bugs from beta test
</commit_message>
<xml_diff>
--- a/assets/field_definitions.xlsx
+++ b/assets/field_definitions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrisbrunet/Documents/School/ManskeLab/metadata_repo/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/columbia/Documents/Chris Brunet/metadata_repo/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C5FFE37-B27C-9E40-801C-D54E6FE28768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10BB1B7C-1E58-8F4A-872A-3D838E7AC052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="16220" xr2:uid="{6E97874C-9E6D-3C4C-92D3-41F01BE707D2}"/>
   </bookViews>
@@ -107,9 +107,6 @@
     <t>height of the participant at the time of the scan in centimeters (integer)</t>
   </si>
   <si>
-    <t>unique id of the study that the participant is taking part in</t>
-  </si>
-  <si>
     <t>date scan was recorded (YYYY-MM-DD)</t>
   </si>
   <si>
@@ -125,9 +122,6 @@
     <t>voxel size in 3 dimensions in milimeters [x_mm, y_mm, z_mm]</t>
   </si>
   <si>
-    <t>file extension of image uploaded</t>
-  </si>
-  <si>
     <t>composite_id</t>
   </si>
   <si>
@@ -143,18 +137,6 @@
     <t>institution</t>
   </si>
   <si>
-    <t>university or organization of the uploading member</t>
-  </si>
-  <si>
-    <t>current medical diagnosis or condition of the participant</t>
-  </si>
-  <si>
-    <t>participant's smoking habits (e.g., current smoker, ex-smoker, never smoked)</t>
-  </si>
-  <si>
-    <t>current medical treatments or therapies the participant is undergoing</t>
-  </si>
-  <si>
     <t>indicates if the participant is taking medications known to alter bone metabolism (e.g., yes/no)</t>
   </si>
   <si>
@@ -167,9 +149,6 @@
     <t>indicates if the participant is currently using or has recently used steroids (e.g., yes/no)</t>
   </si>
   <si>
-    <t>the duration (e.g., in days or months) between this scan and a previous scan for the same participant</t>
-  </si>
-  <si>
     <t>participant's assigned group within the study (e.g., control, treatment, disease subtype)</t>
   </si>
   <si>
@@ -180,6 +159,27 @@
   </si>
   <si>
     <t>a quantitative measure of motion artifact during the scan (e.g., a score from 0-10, or a percentage)</t>
+  </si>
+  <si>
+    <t>participant's smoking habits (e.g., yes/no)</t>
+  </si>
+  <si>
+    <t>current medical treatments or therapies the participant is undergoing (string)</t>
+  </si>
+  <si>
+    <t>university or organization of the uploading member (string)</t>
+  </si>
+  <si>
+    <t>current medical diagnosis or condition of the participant (string)</t>
+  </si>
+  <si>
+    <t>unique id of the study that the participant is taking part in (string)</t>
+  </si>
+  <si>
+    <t>the duration (e.g., in days or months) between this scan and a previous scan for the same participant (string)</t>
+  </si>
+  <si>
+    <t>file extension of image uploaded (string)</t>
   </si>
 </sst>
 </file>
@@ -554,7 +554,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -565,162 +565,162 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -733,15 +733,15 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
         <v>47</v>
@@ -749,7 +749,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
more type checking + bug fixing
</commit_message>
<xml_diff>
--- a/assets/field_definitions.xlsx
+++ b/assets/field_definitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/columbia/Documents/Chris Brunet/metadata_repo/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10BB1B7C-1E58-8F4A-872A-3D838E7AC052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75005CB3-345F-684F-9DD8-D487361503A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="16220" xr2:uid="{6E97874C-9E6D-3C4C-92D3-41F01BE707D2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22340" windowHeight="16220" xr2:uid="{6E97874C-9E6D-3C4C-92D3-41F01BE707D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,15 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>sex_assigned_at_birth</t>
-  </si>
-  <si>
-    <t>weight_kg</t>
-  </si>
-  <si>
     <t>height_cm</t>
   </si>
   <si>
@@ -71,18 +62,12 @@
     <t>steroid_use</t>
   </si>
   <si>
-    <t>study_id</t>
-  </si>
-  <si>
     <t>time_interval_between_scans</t>
   </si>
   <si>
     <t>groups</t>
   </si>
   <si>
-    <t>scan_date</t>
-  </si>
-  <si>
     <t>joint_scanned</t>
   </si>
   <si>
@@ -95,39 +80,15 @@
     <t>file_type</t>
   </si>
   <si>
-    <t>sex of participant assigned at birth (M, F, Other)</t>
-  </si>
-  <si>
-    <t>weight of the participant at the time of the scan in kilograms (float)</t>
-  </si>
-  <si>
-    <t>age of the participant at the time of the scan (integer)</t>
-  </si>
-  <si>
-    <t>height of the participant at the time of the scan in centimeters (integer)</t>
-  </si>
-  <si>
-    <t>date scan was recorded (YYYY-MM-DD)</t>
-  </si>
-  <si>
     <t>length_of_scan_region</t>
   </si>
   <si>
     <t>voxel_spacing</t>
   </si>
   <si>
-    <t>total size of the scan in milimiters in 3 dimensions [x_mm, y_mm, z_mm]</t>
-  </si>
-  <si>
-    <t>voxel size in 3 dimensions in milimeters [x_mm, y_mm, z_mm]</t>
-  </si>
-  <si>
     <t>composite_id</t>
   </si>
   <si>
-    <t>id of scan comprised of participant age, study_id, and scan_date (this field is automatically generated)</t>
-  </si>
-  <si>
     <t>Field</t>
   </si>
   <si>
@@ -137,49 +98,88 @@
     <t>institution</t>
   </si>
   <si>
-    <t>indicates if the participant is taking medications known to alter bone metabolism (e.g., yes/no)</t>
-  </si>
-  <si>
-    <t>indicates if the participant is taking conventional Disease-Modifying Antirheumatic Drugs (DMARDs) (e.g., yes/no)</t>
-  </si>
-  <si>
-    <t>indicates if the participant is taking biological Disease-Modifying Antirheumatic Drugs (DMARDs) (e.g., yes/no)</t>
-  </si>
-  <si>
-    <t>indicates if the participant is currently using or has recently used steroids (e.g., yes/no)</t>
-  </si>
-  <si>
-    <t>participant's assigned group within the study (e.g., control, treatment, disease subtype)</t>
-  </si>
-  <si>
-    <t>specific anatomical joint that was scanned (e.g., right knee, left wrist, lumbar spine)</t>
-  </si>
-  <si>
-    <t>a more detailed description if a hand scan was performed (e.g., dominant hand, specific fingers)</t>
-  </si>
-  <si>
-    <t>a quantitative measure of motion artifact during the scan (e.g., a score from 0-10, or a percentage)</t>
-  </si>
-  <si>
-    <t>participant's smoking habits (e.g., yes/no)</t>
-  </si>
-  <si>
-    <t>current medical treatments or therapies the participant is undergoing (string)</t>
-  </si>
-  <si>
-    <t>university or organization of the uploading member (string)</t>
-  </si>
-  <si>
-    <t>current medical diagnosis or condition of the participant (string)</t>
-  </si>
-  <si>
-    <t>unique id of the study that the participant is taking part in (string)</t>
-  </si>
-  <si>
-    <t>the duration (e.g., in days or months) between this scan and a previous scan for the same participant (string)</t>
-  </si>
-  <si>
-    <t>file extension of image uploaded (string)</t>
+    <t>university or organization of the uploading member (e.g., University of Calgary) : string</t>
+  </si>
+  <si>
+    <t>age of the participant at the time of the scan (e.g., 45) : int</t>
+  </si>
+  <si>
+    <t>sex of participant assigned at birth (e.g., M, F, Other) : string</t>
+  </si>
+  <si>
+    <t>weight of the participant at the time of the scan in kilograms (e.g., 75.2) : float</t>
+  </si>
+  <si>
+    <t>height of the participant at the time of the scan in centimeters (e.g., 185) : int</t>
+  </si>
+  <si>
+    <t>current medical diagnosis or condition of the participant (e.g., OA) : string</t>
+  </si>
+  <si>
+    <t>participant's smoking habits (e.g., Y/N) : string</t>
+  </si>
+  <si>
+    <t>current medical treatments or therapies the participant is undergoing : string</t>
+  </si>
+  <si>
+    <t>indicates if the participant is taking medications known to alter bone metabolism (e.g., Y/N) : string</t>
+  </si>
+  <si>
+    <t>indicates if the participant is currently using or has recently used steroids (e.g., Y/N) : string</t>
+  </si>
+  <si>
+    <t>unique id of the study that the participant is taking part in (e.g., 3300_SPECTRA) : string</t>
+  </si>
+  <si>
+    <t>description of follow up schedule for patients in the study (e.g., BL, FU3mo, FU6mo) : string</t>
+  </si>
+  <si>
+    <t>participant's assigned group within the study (e.g., control, treatment, disease subtype) : string</t>
+  </si>
+  <si>
+    <t>date scan was recorded (YYYY-MM-DD) : date</t>
+  </si>
+  <si>
+    <t>a quantitative measure of motion artifact during the scan (e.g., a score from 0-10) : int</t>
+  </si>
+  <si>
+    <t>a more detailed description if a hand scan was performed (e.g., dominant hand, specific fingers) : string</t>
+  </si>
+  <si>
+    <t>file extension of image uploaded (e.g., .isq, .dcm) : string</t>
+  </si>
+  <si>
+    <t>specific anatomical joint that was scanned (e.g., right knee, left wrist, lumbar spine) : string</t>
+  </si>
+  <si>
+    <t>total size of the scan in milimiters in 3 dimensions [x_mm, y_mm, z_mm] : 1x3 float</t>
+  </si>
+  <si>
+    <t>voxel size in 3 dimensions in milimeters [x_mm, y_mm, z_mm] : 1x3 float</t>
+  </si>
+  <si>
+    <t>id of scan comprised of participant age, study_id, and scan_date (this field is automatically generated) : string</t>
+  </si>
+  <si>
+    <t>indicates if the participant is taking biological Disease-Modifying Antirheumatic Drugs (e.g., Y/N) : string</t>
+  </si>
+  <si>
+    <t>indicates if the participant is taking conventional Disease-Modifying Antirheumatic Drugs (e.g., Y/N) : string</t>
+  </si>
+  <si>
+    <t>age*</t>
+  </si>
+  <si>
+    <t>sex_assigned_at_birth*</t>
+  </si>
+  <si>
+    <t>weight_kg*</t>
+  </si>
+  <si>
+    <t>study_id*</t>
+  </si>
+  <si>
+    <t>scan_date*</t>
   </si>
 </sst>
 </file>
@@ -554,7 +554,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -565,23 +565,23 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
         <v>21</v>
@@ -589,170 +589,170 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>